<commit_message>
add notify when both approve
</commit_message>
<xml_diff>
--- a/packages/backend/public/template/TopicTemplate.xlsx
+++ b/packages/backend/public/template/TopicTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quang\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87099B69-E3C3-458A-B165-9FEC2B551D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C1CF00-7822-49C0-86EF-F2B5888F116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7A374D5C-CBB3-44F8-87FF-81418782261D}"/>
   </bookViews>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>2022-02-20</t>
-  </si>
-  <si>
-    <t>Huynh Xuan Phung</t>
-  </si>
-  <si>
-    <t>0121</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>CODE</t>
   </si>
@@ -59,38 +50,50 @@
     <t>LIMIT</t>
   </si>
   <si>
-    <t>LECTURER NAME</t>
-  </si>
-  <si>
-    <t>DEADLINE</t>
-  </si>
-  <si>
     <t>LECTURER_CODE</t>
   </si>
   <si>
     <t>SCHEDULE</t>
   </si>
   <si>
-    <t>TLCN CNTT</t>
-  </si>
-  <si>
-    <t>HJHJH</t>
-  </si>
-  <si>
     <t>HUDHJDHJ</t>
   </si>
   <si>
     <t>HJSKSGHJK</t>
+  </si>
+  <si>
+    <t>TL-1</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>22-TLCN</t>
+  </si>
+  <si>
+    <t>CRITICAL_CODE</t>
+  </si>
+  <si>
+    <t>2023-01-01</t>
+  </si>
+  <si>
+    <t>THESIS_DEFENSE_DATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,7 +447,7 @@
     <col min="3" max="3" width="32.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.21875" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
@@ -452,57 +455,58 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>